<commit_message>
Goshop Googledrive 1st Commit Rev 0.1
</commit_message>
<xml_diff>
--- a/samuel-tw@outlook.com/products_list.xlsx
+++ b/samuel-tw@outlook.com/products_list.xlsx
@@ -481,12 +481,12 @@
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
+          <t>進貨價</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
           <t>url</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>進貨價</t>
         </is>
       </c>
     </row>
@@ -518,13 +518,13 @@
         </is>
       </c>
       <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr">
+      <c r="J2" t="n">
+        <v>45.15</v>
+      </c>
+      <c r="K2" t="inlineStr">
         <is>
           <t>https://baibaoshop.com/product/bluetooth-large-screen-tws-headset-wireless/</t>
         </is>
-      </c>
-      <c r="K2" t="n">
-        <v>45.15</v>
       </c>
     </row>
     <row r="3">
@@ -555,13 +555,13 @@
         </is>
       </c>
       <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr">
+      <c r="J3" t="n">
+        <v>94.89</v>
+      </c>
+      <c r="K3" t="inlineStr">
         <is>
           <t>https://baibaoshop.com/product/hy300-pro-projector-home-theater-entertainment-portable-small-projector/</t>
         </is>
-      </c>
-      <c r="K3" t="n">
-        <v>94.89</v>
       </c>
     </row>
     <row r="4">
@@ -592,13 +592,13 @@
         </is>
       </c>
       <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr">
+      <c r="J4" t="n">
+        <v>29.73</v>
+      </c>
+      <c r="K4" t="inlineStr">
         <is>
           <t>https://baibaoshop.com/product/hd-sports-camera-dv-hd-portable/</t>
         </is>
-      </c>
-      <c r="K4" t="n">
-        <v>29.73</v>
       </c>
     </row>
     <row r="5">
@@ -629,13 +629,13 @@
         </is>
       </c>
       <c r="I5" t="inlineStr"/>
-      <c r="J5" t="inlineStr">
+      <c r="J5" t="n">
+        <v>32.44</v>
+      </c>
+      <c r="K5" t="inlineStr">
         <is>
           <t>https://baibaoshop.com/product/graffiti-smart-home-bluetooth-finger-robot-app-remote-timing-voice-control-wireless-lamp-artifact/</t>
         </is>
-      </c>
-      <c r="K5" t="n">
-        <v>43.44</v>
       </c>
     </row>
     <row r="6">
@@ -666,13 +666,13 @@
         </is>
       </c>
       <c r="I6" t="inlineStr"/>
-      <c r="J6" t="inlineStr">
+      <c r="J6" t="n">
+        <v>83.42</v>
+      </c>
+      <c r="K6" t="inlineStr">
         <is>
           <t>https://baibaoshop.com/product/headworn-sports-noise-cancelling-bluetooth-earphones/</t>
         </is>
-      </c>
-      <c r="K6" t="n">
-        <v>83.43000000000001</v>
       </c>
     </row>
     <row r="7">
@@ -703,13 +703,13 @@
         </is>
       </c>
       <c r="I7" t="inlineStr"/>
-      <c r="J7" t="inlineStr">
+      <c r="J7" t="n">
+        <v>96.84</v>
+      </c>
+      <c r="K7" t="inlineStr">
         <is>
           <t>https://baibaoshop.com/product/intelligent-programming-spaceman-bluetooth-stereo-dancing-robot/</t>
         </is>
-      </c>
-      <c r="K7" t="n">
-        <v>96.84</v>
       </c>
     </row>
     <row r="8">
@@ -740,13 +740,13 @@
         </is>
       </c>
       <c r="I8" t="inlineStr"/>
-      <c r="J8" t="inlineStr">
+      <c r="J8" t="n">
+        <v>81.73999999999999</v>
+      </c>
+      <c r="K8" t="inlineStr">
         <is>
           <t>https://baibaoshop.com/product/f26-smart-watch-headset-three-in-one-fashion-sports-bracelet/</t>
         </is>
-      </c>
-      <c r="K8" t="n">
-        <v>81.73999999999999</v>
       </c>
     </row>
     <row r="9">
@@ -777,13 +777,13 @@
         </is>
       </c>
       <c r="I9" t="inlineStr"/>
-      <c r="J9" t="inlineStr">
+      <c r="J9" t="n">
+        <v>39.98</v>
+      </c>
+      <c r="K9" t="inlineStr">
         <is>
           <t>https://baibaoshop.com/product/smart-bluetooth-translation-headphones-instant-wireless-headset-language/</t>
         </is>
-      </c>
-      <c r="K9" t="n">
-        <v>39.98</v>
       </c>
     </row>
     <row r="10">
@@ -814,13 +814,13 @@
         </is>
       </c>
       <c r="I10" t="inlineStr"/>
-      <c r="J10" t="inlineStr">
+      <c r="J10" t="n">
+        <v>24.66</v>
+      </c>
+      <c r="K10" t="inlineStr">
         <is>
           <t>https://baibaoshop.com/product/white-noise-sleeping-aid-instrument-soothing-sleep-breathing-table-lamp/</t>
         </is>
-      </c>
-      <c r="K10" t="n">
-        <v>24.66</v>
       </c>
     </row>
     <row r="11">
@@ -851,13 +851,13 @@
         </is>
       </c>
       <c r="I11" t="inlineStr"/>
-      <c r="J11" t="inlineStr">
+      <c r="J11" t="n">
+        <v>136.3</v>
+      </c>
+      <c r="K11" t="inlineStr">
         <is>
           <t>https://baibaoshop.com/product/body-temperature-monitoring-blood-oxygen-heart-rate-breathing-rate-sleep-health-smart-watch/</t>
         </is>
-      </c>
-      <c r="K11" t="n">
-        <v>136.3</v>
       </c>
     </row>
     <row r="12">
@@ -888,13 +888,13 @@
         </is>
       </c>
       <c r="I12" t="inlineStr"/>
-      <c r="J12" t="inlineStr">
+      <c r="J12" t="n">
+        <v>63.56</v>
+      </c>
+      <c r="K12" t="inlineStr">
         <is>
           <t>https://baibaoshop.com/product/square-audio-high-power-portable-subwoofer/</t>
         </is>
-      </c>
-      <c r="K12" t="n">
-        <v>63.56</v>
       </c>
     </row>
     <row r="13">
@@ -925,13 +925,13 @@
         </is>
       </c>
       <c r="I13" t="inlineStr"/>
-      <c r="J13" t="inlineStr">
+      <c r="J13" t="n">
+        <v>30.96</v>
+      </c>
+      <c r="K13" t="inlineStr">
         <is>
           <t>https://baibaoshop.com/product/square-audio-high-power-portable-subwoofer/</t>
         </is>
-      </c>
-      <c r="K13" t="n">
-        <v>30.9</v>
       </c>
     </row>
     <row r="14">
@@ -962,13 +962,13 @@
         </is>
       </c>
       <c r="I14" t="inlineStr"/>
-      <c r="J14" t="inlineStr">
+      <c r="J14" t="n">
+        <v>12.05</v>
+      </c>
+      <c r="K14" t="inlineStr">
         <is>
           <t>https://baibaoshop.com/product/headset-bluetooth-wireless-mobile-phone-music-foldable-running-earphone/</t>
         </is>
-      </c>
-      <c r="K14" t="n">
-        <v>12.05</v>
       </c>
     </row>
     <row r="15">
@@ -999,13 +999,13 @@
         </is>
       </c>
       <c r="I15" t="inlineStr"/>
-      <c r="J15" t="inlineStr">
+      <c r="J15" t="n">
+        <v>72.81999999999999</v>
+      </c>
+      <c r="K15" t="inlineStr">
         <is>
           <t>https://baibaoshop.com/product/solar-battery-low-power-wireless-surveillance-camera/</t>
         </is>
-      </c>
-      <c r="K15" t="n">
-        <v>72.81999999999999</v>
       </c>
     </row>
     <row r="16">
@@ -1036,13 +1036,13 @@
         </is>
       </c>
       <c r="I16" t="inlineStr"/>
-      <c r="J16" t="inlineStr">
+      <c r="J16" t="n">
+        <v>13.88</v>
+      </c>
+      <c r="K16" t="inlineStr">
         <is>
           <t>https://baibaoshop.com/product/microphone-karaoke-machine-bluetooth-speaker-with-2-wireless-mic-rgb-light-home-family-singing-speaker/</t>
         </is>
-      </c>
-      <c r="K16" t="n">
-        <v>13.88</v>
       </c>
     </row>
     <row r="17">
@@ -1073,13 +1073,13 @@
         </is>
       </c>
       <c r="I17" t="inlineStr"/>
-      <c r="J17" t="inlineStr">
+      <c r="J17" t="n">
+        <v>119.04</v>
+      </c>
+      <c r="K17" t="inlineStr">
         <is>
           <t>https://baibaoshop.com/product/projector-home-office-mobile-phone-wireless-hd-projector-portable-overhead-projector-home-theater/</t>
         </is>
-      </c>
-      <c r="K17" t="n">
-        <v>119.04</v>
       </c>
     </row>
     <row r="18">
@@ -1110,13 +1110,13 @@
         </is>
       </c>
       <c r="I18" t="inlineStr"/>
-      <c r="J18" t="inlineStr">
+      <c r="J18" t="n">
+        <v>7.54</v>
+      </c>
+      <c r="K18" t="inlineStr">
         <is>
           <t>https://baibaoshop.com/product/bluetooth-automotive-mp3-player-charger-multi-function-vehicle-mounted-fm-emitter-car-charger-fast-charge/</t>
         </is>
-      </c>
-      <c r="K18" t="n">
-        <v>7.54</v>
       </c>
     </row>
     <row r="19">
@@ -1147,13 +1147,13 @@
         </is>
       </c>
       <c r="I19" t="inlineStr"/>
-      <c r="J19" t="inlineStr">
+      <c r="J19" t="n">
+        <v>13.18</v>
+      </c>
+      <c r="K19" t="inlineStr">
         <is>
           <t>https://baibaoshop.com/product/comes-with-four-wire-three-in-one-solar-charging-unit-digital-display/</t>
         </is>
-      </c>
-      <c r="K19" t="n">
-        <v>13.18</v>
       </c>
     </row>
     <row r="20">
@@ -1184,13 +1184,13 @@
         </is>
       </c>
       <c r="I20" t="inlineStr"/>
-      <c r="J20" t="inlineStr">
+      <c r="J20" t="n">
+        <v>49.43</v>
+      </c>
+      <c r="K20" t="inlineStr">
         <is>
           <t>https://baibaoshop.com/product/childrens-phone-smart-watch-video-gps-positioning-photograph-waterproof-step-counting/</t>
         </is>
-      </c>
-      <c r="K20" t="n">
-        <v>59.43</v>
       </c>
     </row>
     <row r="21">
@@ -1221,13 +1221,13 @@
         </is>
       </c>
       <c r="I21" t="inlineStr"/>
-      <c r="J21" t="inlineStr">
+      <c r="J21" t="n">
+        <v>67.08</v>
+      </c>
+      <c r="K21" t="inlineStr">
         <is>
           <t>https://baibaoshop.com/product/et580-smart-watch-bluetooth-calling-sports/</t>
         </is>
-      </c>
-      <c r="K21" t="n">
-        <v>67.08</v>
       </c>
     </row>
   </sheetData>

</xml_diff>